<commit_message>
fixing spelling of sq.ft from sq.fit
</commit_message>
<xml_diff>
--- a/input/test.xlsx
+++ b/input/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab64e2a4e4af5b78/Documents/Coding Projects/Python/InvoiceGenerator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab64e2a4e4af5b78/Documents/Coding Projects/Python/InvoiceGenerator/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{6528427F-F5E9-4A6C-BD7E-1BB8DAEE3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D03DE97C-0A94-4942-9AC5-64A978B2E4F4}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{6528427F-F5E9-4A6C-BD7E-1BB8DAEE3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC3B7A00-D445-40EB-BB82-B64FF6871A12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9FCCB502-457E-40DE-96DB-A8112C943429}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{9FCCB502-457E-40DE-96DB-A8112C943429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Area, Sq.fit</t>
-  </si>
-  <si>
     <t>Self-occupied</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Area, Sq.ft</t>
   </si>
 </sst>
 </file>
@@ -260,14 +260,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,7 +560,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,34 +579,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -618,19 +614,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5">
         <v>103</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6">
         <v>2045</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6">
         <v>300006</v>
@@ -657,19 +653,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5">
         <v>105</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="6">
         <v>230</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="6">
         <v>20000</v>
@@ -698,19 +694,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>106</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6">
         <v>230</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="6">
         <v>20000</v>

</xml_diff>